<commit_message>
un po' aggiustato un po' rotto
</commit_message>
<xml_diff>
--- a/model/optimization/matlab/opti-ide-val-single-precision.xlsx
+++ b/model/optimization/matlab/opti-ide-val-single-precision.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Il mio Drive\Tesi magistrale\Python\CTM-s\model\optimization\matlab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Documents\Uni\LM II anno\Tesi\python\CTM-s\model\optimization\matlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63E0087-8490-4BCD-B7DA-FBF1BD1D788C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3273D68B-624F-4CE5-B489-76B82949DD75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="360" windowWidth="21480" windowHeight="14745"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Integral delta" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
   <si>
     <t>grado</t>
   </si>
@@ -63,6 +63,240 @@
   </si>
   <si>
     <t>grado</t>
+  </si>
+  <si>
+    <t>SSR_ide</t>
+  </si>
+  <si>
+    <t>SSR_val</t>
+  </si>
+  <si>
+    <t>Val_FPE</t>
+  </si>
+  <si>
+    <t>Val_AIC</t>
+  </si>
+  <si>
+    <t>Val_MDL</t>
+  </si>
+  <si>
+    <t>R2_ide</t>
+  </si>
+  <si>
+    <t>R2a_ide</t>
+  </si>
+  <si>
+    <t>RMSE_ide</t>
+  </si>
+  <si>
+    <t>R2_val</t>
+  </si>
+  <si>
+    <t>R2a_val</t>
+  </si>
+  <si>
+    <t>RMSE_val</t>
+  </si>
+  <si>
+    <t>grado</t>
+  </si>
+  <si>
+    <t>tol</t>
+  </si>
+  <si>
+    <t>SSR_ide</t>
+  </si>
+  <si>
+    <t>SSR_val</t>
+  </si>
+  <si>
+    <t>Val_FPE</t>
+  </si>
+  <si>
+    <t>Val_AIC</t>
+  </si>
+  <si>
+    <t>Val_MDL</t>
+  </si>
+  <si>
+    <t>R2_ide</t>
+  </si>
+  <si>
+    <t>R2a_ide</t>
+  </si>
+  <si>
+    <t>RMSE_ide</t>
+  </si>
+  <si>
+    <t>R2_val</t>
+  </si>
+  <si>
+    <t>R2a_val</t>
+  </si>
+  <si>
+    <t>RMSE_val</t>
+  </si>
+  <si>
+    <t>grado</t>
+  </si>
+  <si>
+    <t>tol</t>
+  </si>
+  <si>
+    <t>SSR_ide</t>
+  </si>
+  <si>
+    <t>SSR_val</t>
+  </si>
+  <si>
+    <t>Val_FPE</t>
+  </si>
+  <si>
+    <t>Val_AIC</t>
+  </si>
+  <si>
+    <t>Val_MDL</t>
+  </si>
+  <si>
+    <t>R2_ide</t>
+  </si>
+  <si>
+    <t>R2a_ide</t>
+  </si>
+  <si>
+    <t>RMSE_ide</t>
+  </si>
+  <si>
+    <t>R2_val</t>
+  </si>
+  <si>
+    <t>R2a_val</t>
+  </si>
+  <si>
+    <t>RMSE_val</t>
+  </si>
+  <si>
+    <t>grado</t>
+  </si>
+  <si>
+    <t>tol</t>
+  </si>
+  <si>
+    <t>SSR_ide</t>
+  </si>
+  <si>
+    <t>SSR_val</t>
+  </si>
+  <si>
+    <t>Val_FPE</t>
+  </si>
+  <si>
+    <t>Val_AIC</t>
+  </si>
+  <si>
+    <t>Val_MDL</t>
+  </si>
+  <si>
+    <t>R2_ide</t>
+  </si>
+  <si>
+    <t>R2a_ide</t>
+  </si>
+  <si>
+    <t>RMSE_ide</t>
+  </si>
+  <si>
+    <t>R2_val</t>
+  </si>
+  <si>
+    <t>R2a_val</t>
+  </si>
+  <si>
+    <t>RMSE_val</t>
+  </si>
+  <si>
+    <t>grado</t>
+  </si>
+  <si>
+    <t>tol</t>
+  </si>
+  <si>
+    <t>SSR_ide</t>
+  </si>
+  <si>
+    <t>SSR_val</t>
+  </si>
+  <si>
+    <t>Val_FPE</t>
+  </si>
+  <si>
+    <t>Val_AIC</t>
+  </si>
+  <si>
+    <t>Val_MDL</t>
+  </si>
+  <si>
+    <t>R2_ide</t>
+  </si>
+  <si>
+    <t>R2a_ide</t>
+  </si>
+  <si>
+    <t>RMSE_ide</t>
+  </si>
+  <si>
+    <t>R2_val</t>
+  </si>
+  <si>
+    <t>R2a_val</t>
+  </si>
+  <si>
+    <t>RMSE_val</t>
+  </si>
+  <si>
+    <t>grado</t>
+  </si>
+  <si>
+    <t>tol</t>
+  </si>
+  <si>
+    <t>SSR_ide</t>
+  </si>
+  <si>
+    <t>SSR_val</t>
+  </si>
+  <si>
+    <t>Val_FPE</t>
+  </si>
+  <si>
+    <t>Val_AIC</t>
+  </si>
+  <si>
+    <t>Val_MDL</t>
+  </si>
+  <si>
+    <t>R2_ide</t>
+  </si>
+  <si>
+    <t>R2a_ide</t>
+  </si>
+  <si>
+    <t>RMSE_ide</t>
+  </si>
+  <si>
+    <t>R2_val</t>
+  </si>
+  <si>
+    <t>R2a_val</t>
+  </si>
+  <si>
+    <t>RMSE_val</t>
+  </si>
+  <si>
+    <t>grado</t>
+  </si>
+  <si>
+    <t>tol</t>
   </si>
   <si>
     <t>SSR_ide</t>
@@ -572,55 +806,50 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.140625" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="15.85546875" customWidth="true"/>
-    <col min="5" max="5" width="11.7109375" customWidth="true"/>
-    <col min="7" max="7" width="12.7109375" customWidth="true"/>
+    <col min="2" max="4" width="15.85546875" customWidth="true"/>
+    <col min="5" max="6" width="11.7109375" customWidth="true"/>
+    <col min="7" max="8" width="12.7109375" customWidth="true"/>
     <col min="9" max="9" width="11.7109375" customWidth="true"/>
-    <col min="10" max="10" width="12.7109375" customWidth="true"/>
+    <col min="10" max="11" width="12.7109375" customWidth="true"/>
     <col min="12" max="12" width="11.7109375" customWidth="true"/>
-    <col min="3" max="3" width="15.85546875" customWidth="true"/>
-    <col min="4" max="4" width="15.85546875" customWidth="true"/>
-    <col min="6" max="6" width="11.7109375" customWidth="true"/>
-    <col min="8" max="8" width="12.7109375" customWidth="true"/>
-    <col min="11" max="11" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>23</v>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2">
@@ -1042,40 +1271,40 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="0">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="0">
+      <c r="B13">
         <v>188901851136</v>
       </c>
-      <c r="C13" s="0">
+      <c r="C13">
         <v>34459783168</v>
       </c>
-      <c r="D13" s="0">
+      <c r="D13">
         <v>191622103040</v>
       </c>
-      <c r="E13" s="0">
+      <c r="E13">
         <v>25.978790283203125</v>
       </c>
-      <c r="F13" s="0">
+      <c r="F13">
         <v>26.053476333618164</v>
       </c>
-      <c r="G13" s="0">
+      <c r="G13">
         <v>0.52575081586837769</v>
       </c>
-      <c r="H13" s="0">
+      <c r="H13">
         <v>0.52233803272247314</v>
       </c>
-      <c r="I13" s="0">
+      <c r="I13">
         <v>859.11737060546875</v>
       </c>
-      <c r="J13" s="0">
+      <c r="J13">
         <v>0.50397318601608276</v>
       </c>
-      <c r="K13" s="0">
+      <c r="K13">
         <v>0.48304265737533569</v>
       </c>
-      <c r="L13" s="0">
+      <c r="L13">
         <v>874.75543212890625</v>
       </c>
     </row>
@@ -1111,43 +1340,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>50</v>
+        <v>128</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>52</v>
+        <v>130</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>53</v>
+        <v>131</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>54</v>
+        <v>132</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>55</v>
+        <v>133</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>56</v>
+        <v>134</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>57</v>
+        <v>135</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>58</v>
+        <v>136</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>59</v>
+        <v>137</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>60</v>
+        <v>138</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>61</v>
+        <v>139</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2">
@@ -1155,40 +1384,40 @@
         <v>8</v>
       </c>
       <c r="B2" s="0">
-        <v>9.9999997473787516e-06</v>
+        <v>0.10000000149011612</v>
       </c>
       <c r="C2" s="0">
-        <v>178953912320</v>
+        <v>180454424576</v>
       </c>
       <c r="D2" s="0">
-        <v>30845911040</v>
+        <v>31225214976</v>
       </c>
       <c r="E2" s="0">
-        <v>179495960576</v>
+        <v>180826210304</v>
       </c>
       <c r="F2" s="0">
-        <v>25.913419723510742</v>
+        <v>25.920801162719727</v>
       </c>
       <c r="G2" s="0">
-        <v>25.929218292236328</v>
+        <v>25.931552886962891</v>
       </c>
       <c r="H2" s="0">
-        <v>0.54834675788879395</v>
+        <v>0.54455399513244629</v>
       </c>
       <c r="I2" s="0">
-        <v>0.54766452312469482</v>
+        <v>0.54408657550811768</v>
       </c>
       <c r="J2" s="0">
-        <v>838.40093994140625</v>
+        <v>841.9139404296875</v>
       </c>
       <c r="K2" s="0">
-        <v>0.55493974685668945</v>
+        <v>0.54947173595428467</v>
       </c>
       <c r="L2" s="0">
-        <v>0.55110293626785278</v>
+        <v>0.54683911800384521</v>
       </c>
       <c r="M2" s="0">
-        <v>828.59716796875</v>
+        <v>833.67138671875</v>
       </c>
     </row>
     <row r="3">
@@ -1196,40 +1425,40 @@
         <v>8</v>
       </c>
       <c r="B3" s="0">
-        <v>10</v>
+        <v>0.0099999997764825821</v>
       </c>
       <c r="C3" s="0">
-        <v>189840818176</v>
+        <v>181130248192</v>
       </c>
       <c r="D3" s="0">
-        <v>32744464384</v>
+        <v>31335268352</v>
       </c>
       <c r="E3" s="0">
-        <v>190121394176</v>
+        <v>181479194624</v>
       </c>
       <c r="F3" s="0">
-        <v>25.970928192138672</v>
+        <v>25.924406051635742</v>
       </c>
       <c r="G3" s="0">
-        <v>25.978643417358398</v>
+        <v>25.934459686279297</v>
       </c>
       <c r="H3" s="0">
-        <v>0.52086985111236572</v>
+        <v>0.54285407066345215</v>
       </c>
       <c r="I3" s="0">
-        <v>0.52051770687103271</v>
+        <v>0.54241549968719482</v>
       </c>
       <c r="J3" s="0">
-        <v>863.52703857421875</v>
+        <v>843.48358154296875</v>
       </c>
       <c r="K3" s="0">
-        <v>0.52753531932830811</v>
+        <v>0.5478670597076416</v>
       </c>
       <c r="L3" s="0">
-        <v>0.52556055784225464</v>
+        <v>0.54539811611175537</v>
       </c>
       <c r="M3" s="0">
-        <v>853.72576904296875</v>
+        <v>835.154541015625</v>
       </c>
     </row>
     <row r="4">
@@ -1237,40 +1466,40 @@
         <v>8</v>
       </c>
       <c r="B4" s="0">
-        <v>100</v>
+        <v>0.0010000000474974513</v>
       </c>
       <c r="C4" s="0">
-        <v>196140072960</v>
+        <v>181130231808</v>
       </c>
       <c r="D4" s="0">
-        <v>33993496576</v>
+        <v>31335268352</v>
       </c>
       <c r="E4" s="0">
-        <v>196365156352</v>
+        <v>181479178240</v>
       </c>
       <c r="F4" s="0">
-        <v>26.003240585327148</v>
+        <v>25.924406051635742</v>
       </c>
       <c r="G4" s="0">
-        <v>26.009231567382813</v>
+        <v>25.934459686279297</v>
       </c>
       <c r="H4" s="0">
-        <v>0.50498604774475098</v>
+        <v>0.54285407066345215</v>
       </c>
       <c r="I4" s="0">
-        <v>0.50470399856567383</v>
+        <v>0.54241549968719482</v>
       </c>
       <c r="J4" s="0">
-        <v>877.723876953125</v>
+        <v>843.48358154296875</v>
       </c>
       <c r="K4" s="0">
-        <v>0.50953871011734009</v>
+        <v>0.5478670597076416</v>
       </c>
       <c r="L4" s="0">
-        <v>0.50795066356658936</v>
+        <v>0.54539811611175537</v>
       </c>
       <c r="M4" s="0">
-        <v>869.83404541015625</v>
+        <v>835.154541015625</v>
       </c>
     </row>
     <row r="5">
@@ -1278,40 +1507,40 @@
         <v>8</v>
       </c>
       <c r="B5" s="0">
-        <v>1000</v>
+        <v>9.9999997473787516e-05</v>
       </c>
       <c r="C5" s="0">
-        <v>206905458688</v>
+        <v>181130231808</v>
       </c>
       <c r="D5" s="0">
-        <v>35839303680</v>
+        <v>31335266304</v>
       </c>
       <c r="E5" s="0">
-        <v>207094087680</v>
+        <v>181479178240</v>
       </c>
       <c r="F5" s="0">
-        <v>26.056440353393555</v>
+        <v>25.924406051635742</v>
       </c>
       <c r="G5" s="0">
-        <v>26.061199188232422</v>
+        <v>25.934459686279297</v>
       </c>
       <c r="H5" s="0">
-        <v>0.47780746221542358</v>
+        <v>0.54285407066345215</v>
       </c>
       <c r="I5" s="0">
-        <v>0.47757148742675781</v>
+        <v>0.54241549968719482</v>
       </c>
       <c r="J5" s="0">
-        <v>901.49755859375</v>
+        <v>843.48358154296875</v>
       </c>
       <c r="K5" s="0">
-        <v>0.48290395736694336</v>
+        <v>0.5478670597076416</v>
       </c>
       <c r="L5" s="0">
-        <v>0.48157691955566406</v>
+        <v>0.54539811611175537</v>
       </c>
       <c r="M5" s="0">
-        <v>893.1407470703125</v>
+        <v>835.154541015625</v>
       </c>
     </row>
     <row r="6">
@@ -1319,40 +1548,40 @@
         <v>8</v>
       </c>
       <c r="B6" s="0">
-        <v>10000</v>
+        <v>9.9999997473787516e-06</v>
       </c>
       <c r="C6" s="0">
-        <v>227120791552</v>
+        <v>181130231808</v>
       </c>
       <c r="D6" s="0">
-        <v>39455596544</v>
+        <v>31335249920</v>
       </c>
       <c r="E6" s="0">
-        <v>227268935680</v>
+        <v>181479178240</v>
       </c>
       <c r="F6" s="0">
-        <v>26.14940071105957</v>
+        <v>25.924406051635742</v>
       </c>
       <c r="G6" s="0">
-        <v>26.152807235717773</v>
+        <v>25.934459686279297</v>
       </c>
       <c r="H6" s="0">
-        <v>0.42678743600845337</v>
+        <v>0.54285407066345215</v>
       </c>
       <c r="I6" s="0">
-        <v>0.42660278081893921</v>
+        <v>0.54241549968719482</v>
       </c>
       <c r="J6" s="0">
-        <v>944.51116943359375</v>
+        <v>843.48358154296875</v>
       </c>
       <c r="K6" s="0">
-        <v>0.43072706460952759</v>
+        <v>0.5478670597076416</v>
       </c>
       <c r="L6" s="0">
-        <v>0.42968612909317017</v>
+        <v>0.54539811611175537</v>
       </c>
       <c r="M6" s="0">
-        <v>937.11761474609375</v>
+        <v>835.154541015625</v>
       </c>
     </row>
     <row r="7">
@@ -1360,40 +1589,40 @@
         <v>8</v>
       </c>
       <c r="B7" s="0">
-        <v>100000</v>
+        <v>9.9999999747524271e-07</v>
       </c>
       <c r="C7" s="0">
-        <v>245071642624</v>
+        <v>181130248192</v>
       </c>
       <c r="D7" s="0">
-        <v>42229440512</v>
+        <v>31335268352</v>
       </c>
       <c r="E7" s="0">
-        <v>245181399040</v>
+        <v>181479194624</v>
       </c>
       <c r="F7" s="0">
-        <v>26.225265502929688</v>
+        <v>25.924406051635742</v>
       </c>
       <c r="G7" s="0">
-        <v>26.227603912353516</v>
+        <v>25.934459686279297</v>
       </c>
       <c r="H7" s="0">
-        <v>0.87358790636062622</v>
+        <v>0.54285407066345215</v>
       </c>
       <c r="I7" s="0">
-        <v>0.87355959415435791</v>
+        <v>0.54241549968719482</v>
       </c>
       <c r="J7" s="0">
-        <v>981.1258544921875</v>
+        <v>843.48358154296875</v>
       </c>
       <c r="K7" s="0">
-        <v>0.87602639198303223</v>
+        <v>0.5478670597076416</v>
       </c>
       <c r="L7" s="0">
-        <v>0.87586891651153564</v>
+        <v>0.54539811611175537</v>
       </c>
       <c r="M7" s="0">
-        <v>969.5159912109375</v>
+        <v>835.154541015625</v>
       </c>
     </row>
     <row r="8">
@@ -1401,40 +1630,40 @@
         <v>8</v>
       </c>
       <c r="B8" s="0">
-        <v>1000000</v>
+        <v>1.0000000116860974e-07</v>
       </c>
       <c r="C8" s="0">
-        <v>347943206912</v>
+        <v>181130248192</v>
       </c>
       <c r="D8" s="0">
-        <v>55449296896</v>
+        <v>31335251968</v>
       </c>
       <c r="E8" s="0">
-        <v>348044361728</v>
+        <v>181479194624</v>
       </c>
       <c r="F8" s="0">
-        <v>26.575595855712891</v>
+        <v>25.924406051635742</v>
       </c>
       <c r="G8" s="0">
-        <v>26.577114105224609</v>
+        <v>25.934459686279297</v>
       </c>
       <c r="H8" s="0">
-        <v>0.82053035497665405</v>
+        <v>0.54285407066345215</v>
       </c>
       <c r="I8" s="0">
-        <v>0.82050424814224243</v>
+        <v>0.54241549968719482</v>
       </c>
       <c r="J8" s="0">
-        <v>1169.0306396484375</v>
+        <v>843.48358154296875</v>
       </c>
       <c r="K8" s="0">
-        <v>0.83727145195007324</v>
+        <v>0.5478670597076416</v>
       </c>
       <c r="L8" s="0">
-        <v>0.83713734149932861</v>
+        <v>0.54539811611175537</v>
       </c>
       <c r="M8" s="0">
-        <v>1110.7650146484375</v>
+        <v>835.154541015625</v>
       </c>
     </row>
     <row r="9">
@@ -1442,40 +1671,40 @@
         <v>8</v>
       </c>
       <c r="B9" s="0">
-        <v>10000000</v>
+        <v>9.9999999392252903e-09</v>
       </c>
       <c r="C9" s="0">
-        <v>515430875136</v>
+        <v>181130248192</v>
       </c>
       <c r="D9" s="0">
-        <v>87026360320</v>
+        <v>31335268352</v>
       </c>
       <c r="E9" s="0">
-        <v>515519971328</v>
+        <v>181479194624</v>
       </c>
       <c r="F9" s="0">
-        <v>26.968442916870117</v>
+        <v>25.924406051635742</v>
       </c>
       <c r="G9" s="0">
-        <v>26.969345092773438</v>
+        <v>25.934459686279297</v>
       </c>
       <c r="H9" s="0">
-        <v>0.73420196771621704</v>
+        <v>0.54285407066345215</v>
       </c>
       <c r="I9" s="0">
-        <v>0.73417901992797852</v>
+        <v>0.54241549968719482</v>
       </c>
       <c r="J9" s="0">
-        <v>1422.677001953125</v>
+        <v>843.48358154296875</v>
       </c>
       <c r="K9" s="0">
-        <v>0.74455356597900391</v>
+        <v>0.5478670597076416</v>
       </c>
       <c r="L9" s="0">
-        <v>0.74442839622497559</v>
+        <v>0.54539811611175537</v>
       </c>
       <c r="M9" s="0">
-        <v>1391.6822509765625</v>
+        <v>835.154541015625</v>
       </c>
     </row>
     <row r="10">
@@ -1483,40 +1712,40 @@
         <v>8</v>
       </c>
       <c r="B10" s="0">
-        <v>100000000</v>
+        <v>9.9999997171806854e-10</v>
       </c>
       <c r="C10" s="0">
-        <v>714940874752</v>
+        <v>181130248192</v>
       </c>
       <c r="D10" s="0">
-        <v>124265963520</v>
+        <v>31335266304</v>
       </c>
       <c r="E10" s="0">
-        <v>715013881856</v>
+        <v>181479194624</v>
       </c>
       <c r="F10" s="0">
-        <v>27.295568466186523</v>
+        <v>25.924406051635742</v>
       </c>
       <c r="G10" s="0">
-        <v>27.296100616455078</v>
+        <v>25.934459686279297</v>
       </c>
       <c r="H10" s="0">
-        <v>0.6312137246131897</v>
+        <v>0.54285407066345215</v>
       </c>
       <c r="I10" s="0">
-        <v>0.63119488954544067</v>
+        <v>0.54241549968719482</v>
       </c>
       <c r="J10" s="0">
-        <v>1675.7828369140625</v>
+        <v>843.48358154296875</v>
       </c>
       <c r="K10" s="0">
-        <v>0.63521099090576172</v>
+        <v>0.5478670597076416</v>
       </c>
       <c r="L10" s="0">
-        <v>0.63510537147521973</v>
+        <v>0.54539811611175537</v>
       </c>
       <c r="M10" s="0">
-        <v>1663.07373046875</v>
+        <v>835.154541015625</v>
       </c>
     </row>
     <row r="11">
@@ -1524,40 +1753,40 @@
         <v>8</v>
       </c>
       <c r="B11" s="0">
-        <v>1000000000</v>
+        <v>1.000000013351432e-10</v>
       </c>
       <c r="C11" s="0">
-        <v>1237432532992</v>
+        <v>181130231808</v>
       </c>
       <c r="D11" s="0">
-        <v>218090012672</v>
+        <v>31335266304</v>
       </c>
       <c r="E11" s="0">
-        <v>1237500559360</v>
+        <v>181479178240</v>
       </c>
       <c r="F11" s="0">
-        <v>27.844114303588867</v>
+        <v>25.924406051635742</v>
       </c>
       <c r="G11" s="0">
-        <v>27.844400405883789</v>
+        <v>25.934459686279297</v>
       </c>
       <c r="H11" s="0">
-        <v>0.36171352863311768</v>
+        <v>0.54285407066345215</v>
       </c>
       <c r="I11" s="0">
-        <v>0.36169600486755371</v>
+        <v>0.54241549968719482</v>
       </c>
       <c r="J11" s="0">
-        <v>2204.642822265625</v>
+        <v>843.48358154296875</v>
       </c>
       <c r="K11" s="0">
-        <v>0.35976803302764893</v>
+        <v>0.5478670597076416</v>
       </c>
       <c r="L11" s="0">
-        <v>0.35966825485229492</v>
+        <v>0.54539811611175537</v>
       </c>
       <c r="M11" s="0">
-        <v>2203.2236328125</v>
+        <v>835.154541015625</v>
       </c>
     </row>
     <row r="12">
@@ -1565,40 +1794,40 @@
         <v>8</v>
       </c>
       <c r="B12" s="0">
-        <v>10000000000</v>
+        <v>0.10000000149011612</v>
       </c>
       <c r="C12" s="0">
-        <v>1530506772480</v>
+        <v>202506731520</v>
       </c>
       <c r="D12" s="0">
-        <v>269238075392</v>
+        <v>35024863232</v>
       </c>
       <c r="E12" s="0">
-        <v>1530530758656</v>
+        <v>202707271680</v>
       </c>
       <c r="F12" s="0">
-        <v>28.056634902954102</v>
+        <v>26.035028457641602</v>
       </c>
       <c r="G12" s="0">
-        <v>28.056716918945313</v>
+        <v>26.040199279785156</v>
       </c>
       <c r="H12" s="0">
-        <v>0.2105410099029541</v>
+        <v>0.48891419172286987</v>
       </c>
       <c r="I12" s="0">
-        <v>0.21053481101989746</v>
+        <v>0.48866313695907593</v>
       </c>
       <c r="J12" s="0">
-        <v>2451.857421875</v>
+        <v>891.85888671875</v>
       </c>
       <c r="K12" s="0">
-        <v>0.20961582660675049</v>
+        <v>0.49465566873550415</v>
       </c>
       <c r="L12" s="0">
-        <v>0.20958065986633301</v>
+        <v>0.49324572086334229</v>
       </c>
       <c r="M12" s="0">
-        <v>2447.987548828125</v>
+        <v>882.93341064453125</v>
       </c>
     </row>
     <row r="13">
@@ -1606,40 +1835,40 @@
         <v>8</v>
       </c>
       <c r="B13" s="0">
-        <v>10000000000</v>
+        <v>0.10000000149011612</v>
       </c>
       <c r="C13" s="0">
-        <v>1530506772480</v>
+        <v>179934314496</v>
       </c>
       <c r="D13" s="0">
-        <v>269238075392</v>
+        <v>31132344320</v>
       </c>
       <c r="E13" s="0">
-        <v>1530530758656</v>
+        <v>180305035264</v>
       </c>
       <c r="F13" s="0">
-        <v>28.056634902954102</v>
+        <v>25.917915344238281</v>
       </c>
       <c r="G13" s="0">
-        <v>28.056716918945313</v>
+        <v>25.928667068481445</v>
       </c>
       <c r="H13" s="0">
-        <v>0.2105410099029541</v>
+        <v>0.54590988159179688</v>
       </c>
       <c r="I13" s="0">
-        <v>0.21053481101989746</v>
+        <v>0.54544389247894287</v>
       </c>
       <c r="J13" s="0">
-        <v>2451.857421875</v>
+        <v>840.6595458984375</v>
       </c>
       <c r="K13" s="0">
-        <v>0.20961582660675049</v>
+        <v>0.55089980363845825</v>
       </c>
       <c r="L13" s="0">
-        <v>0.20958065986633301</v>
+        <v>0.54827553033828735</v>
       </c>
       <c r="M13" s="0">
-        <v>2447.987548828125</v>
+        <v>832.34869384765625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>